<commit_message>
doc: add aivisual per cities links with air sensor station details
</commit_message>
<xml_diff>
--- a/aqi us data recap 07 12 2023.xlsx
+++ b/aqi us data recap 07 12 2023.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aldi Andalan\Documents\revou\polution-daily-backup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{655CAF26-0B1C-4C4D-A43B-C30566D55491}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B753EDC-797E-4C5B-940A-CB634EA66C09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-12" yWindow="0" windowWidth="12150" windowHeight="11760" firstSheet="1" activeTab="1" xr2:uid="{8A0724AA-3800-447E-BE7E-7C1081E679CD}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" firstSheet="1" activeTab="1" xr2:uid="{8A0724AA-3800-447E-BE7E-7C1081E679CD}"/>
   </bookViews>
   <sheets>
     <sheet name="City State Country for URL" sheetId="3" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="643" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="717" uniqueCount="289">
   <si>
     <t>// City State Country Timestamp(ts) AQIUS(aqius)</t>
   </si>
@@ -717,13 +717,190 @@
   </si>
   <si>
     <t>NewAQIUS(aqius)2</t>
+  </si>
+  <si>
+    <t>https://www.iqair.com/id/indonesia/west-java/bandung</t>
+  </si>
+  <si>
+    <t>Airvisual page</t>
+  </si>
+  <si>
+    <t>https://www.iqair.com/id/indonesia/east-java/surabaya</t>
+  </si>
+  <si>
+    <t>https://www.iqair.com/id/indonesia/west-java/depok</t>
+  </si>
+  <si>
+    <t>https://www.iqair.com/id/indonesia/west-java/bekasi</t>
+  </si>
+  <si>
+    <t>https://www.iqair.com/id/indonesia/south-sulawesi/makassar</t>
+  </si>
+  <si>
+    <t>https://www.iqair.com/id/indonesia/south-sumatra/palembang</t>
+  </si>
+  <si>
+    <t>https://www.iqair.com/id/indonesia/riau-islands/batam</t>
+  </si>
+  <si>
+    <t>https://www.iqair.com/id/indonesia/west-kalimantan/pontianak</t>
+  </si>
+  <si>
+    <t>https://www.iqair.com/id/indonesia/west-java/bogor</t>
+  </si>
+  <si>
+    <t>https://www.iqair.com/id/indonesia/central-java/semarang</t>
+  </si>
+  <si>
+    <t>https://www.iqair.com/id/indonesia/east-java/malang</t>
+  </si>
+  <si>
+    <t>https://www.iqair.com/id/indonesia/southeast-sulawesi/kendari</t>
+  </si>
+  <si>
+    <t>https://www.iqair.com/id/indonesia/west-papua/sorong</t>
+  </si>
+  <si>
+    <t>https://www.iqair.com/id/indonesia/west-papua/manokwari</t>
+  </si>
+  <si>
+    <t>Air Censor Station</t>
+  </si>
+  <si>
+    <t>KLHK, LMJAELANI.com, RespoKare Mask Stations</t>
+  </si>
+  <si>
+    <t>RespoKare Mask Setrasari, TMLEnergy, Setra Duta, jalan Sukawarna Baru A Stations</t>
+  </si>
+  <si>
+    <t>https://www.iqair.com/indonesia/north-sumatra/medan/dlh-medan-02</t>
+  </si>
+  <si>
+    <t>https://www.iqair.com/id/indonesia/jakarta</t>
+  </si>
+  <si>
+    <t>https://www.iqair.com/indonesia/yogyakarta/sleman/sleman-station https://www.iqair.com/id/indonesia/yogyakarta</t>
+  </si>
+  <si>
+    <t>https://www.iqair.com/id/indonesia/bali/denpasar</t>
+  </si>
+  <si>
+    <t>https://www.iqair.com/id/indonesia/east-nusa-tenggaara/kupang</t>
+  </si>
+  <si>
+    <t>https://www.iqair.com/id/indonesia/west-nusa-tenggara/mataram</t>
+  </si>
+  <si>
+    <t>https://www.iqair.com/id/indonesia/riau/pekanbaru</t>
+  </si>
+  <si>
+    <t>https://www.iqair.com/id/indonesia/banten/south-tangerang</t>
+  </si>
+  <si>
+    <t>https://www.iqair.com/id/indonesia/banten/serang</t>
+  </si>
+  <si>
+    <t>https://www.iqair.com/id/indonesia/south-kalimantan/banjarbaru/banjarbaru-s</t>
+  </si>
+  <si>
+    <t>https://www.iqair.com/id/indonesia/east-kalimantan/city-of-balikpapan/balikpapan-sepinggan</t>
+  </si>
+  <si>
+    <t>https://www.iqair.com/id/indonesia/east-kalimantan/samarinda/samarinda-s</t>
+  </si>
+  <si>
+    <t>https://www.iqair.com/id/indonesia/bali/ubud/ubudcare-clinic https://www.iqair.com/id/indonesia/bali/ubud/jalan-raya-mas</t>
+  </si>
+  <si>
+    <t>https://www.iqair.com/id/indonesia/bali/badung/east-java-co-bali</t>
+  </si>
+  <si>
+    <t>https://www.iqair.com/id/indonesia/bali/buleleng</t>
+  </si>
+  <si>
+    <t>https://www.iqair.com/id/indonesia/banten/tangerang</t>
+  </si>
+  <si>
+    <t>https://www.iqair.com/id/indonesia/maluku/ambon</t>
+  </si>
+  <si>
+    <t>https://www.iqair.com/id/indonesia/papua/jayapura</t>
+  </si>
+  <si>
+    <t>https://www.iqair.com/id/indonesia/riau/dumai/dumai-bukit-kapur</t>
+  </si>
+  <si>
+    <t>https://www.iqair.com/id/indonesia/maluku/kota-ternate</t>
+  </si>
+  <si>
+    <t>https://www.iqair.com/id/indonesia/aceh/banda-aceh/aceh-syiah-kuala</t>
+  </si>
+  <si>
+    <t>https://www.iqair.com/id/indonesia/riau-islands/tanjung-pinang/tanjung-pinang-taman-pamedan</t>
+  </si>
+  <si>
+    <t>KLHK</t>
+  </si>
+  <si>
+    <t>BMKG</t>
+  </si>
+  <si>
+    <t>KLHK, BMKG</t>
+  </si>
+  <si>
+    <t>Puretrex Indonesia, Green Movement</t>
+  </si>
+  <si>
+    <t>Plataran Menjangan Resort &amp; Spa</t>
+  </si>
+  <si>
+    <t>East Java &amp; Co</t>
+  </si>
+  <si>
+    <t>Anonim, PurpleAir</t>
+  </si>
+  <si>
+    <t>KLHK, PT Barito Pacific Tbk. (BRPT), RespoKare Mask</t>
+  </si>
+  <si>
+    <t>BMKG, KLHK</t>
+  </si>
+  <si>
+    <t>Pesantren Bayt Al-Quran, Inti Garda Pratam, Pakis, Yerun, Yayasan AHP</t>
+  </si>
+  <si>
+    <t>BMKG, KLHK, Kimteng Coffee Company Stations</t>
+  </si>
+  <si>
+    <t>BMKG, KLHK, Hen San</t>
+  </si>
+  <si>
+    <t>BMKG, KLHK, RespoKare Mask</t>
+  </si>
+  <si>
+    <t>Pontiudar Anonim</t>
+  </si>
+  <si>
+    <t>RespoKare Mask Ruko Metro Square</t>
+  </si>
+  <si>
+    <t>KLHK, BMKG + Other 38 Stations</t>
+  </si>
+  <si>
+    <t>PT. Cakra Anugerah Jaya</t>
+  </si>
+  <si>
+    <t>KLHK + Lumi Clinic, Smart Energy Technology, nasi_goreng_87</t>
+  </si>
+  <si>
+    <t>DLH Medan 02, KLHK</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -736,6 +913,14 @@
       <color rgb="FF6A9955"/>
       <name val="Consolas"/>
       <family val="3"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -773,8 +958,9 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -785,11 +971,12 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1308,7 +1495,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23602D85-EE67-4AEF-8112-78B22B43DE7C}">
-  <dimension ref="A1:O37"/>
+  <dimension ref="A1:Q37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
   </sheetViews>
@@ -1323,14 +1510,16 @@
     <col min="8" max="8" width="38.47265625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.68359375" customWidth="1"/>
     <col min="10" max="10" width="10.26171875" customWidth="1"/>
-    <col min="11" max="11" width="35.20703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.83984375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.5234375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="35.5234375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.3125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="35.20703125" customWidth="1"/>
+    <col min="12" max="12" width="15.83984375" customWidth="1"/>
+    <col min="13" max="13" width="11.5234375" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="35.5234375" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="15.3125" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="54" customWidth="1"/>
+    <col min="17" max="17" width="86.41796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>217</v>
       </c>
@@ -1376,12 +1565,18 @@
       <c r="O1" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="P1" t="s">
+        <v>231</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C2" s="3" t="s">
@@ -1423,12 +1618,18 @@
       <c r="O2" s="3" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="P2" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="3">
         <v>2</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C3" s="3" t="s">
@@ -1470,12 +1671,18 @@
       <c r="O3" s="3" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="P3" s="6" t="s">
+        <v>232</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="3">
         <v>3</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C4" s="3" t="s">
@@ -1517,12 +1724,18 @@
       <c r="O4" s="3" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="P4" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="3">
         <v>4</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C5" s="3" t="s">
@@ -1564,12 +1777,18 @@
       <c r="O5" s="3" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="P5" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="Q5" s="2" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="3">
         <v>5</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C6" s="3" t="s">
@@ -1611,12 +1830,18 @@
       <c r="O6" s="3" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="P6" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="Q6" s="2" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="4">
         <v>6</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C7" s="4" t="s">
@@ -1658,12 +1883,18 @@
       <c r="O7" s="4" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="P7" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="4">
         <v>7</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C8" s="4" t="s">
@@ -1705,12 +1936,18 @@
       <c r="O8" s="4" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="P8" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="Q8" s="2" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="5">
         <v>8</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C9" s="5" t="s">
@@ -1752,8 +1989,14 @@
       <c r="O9" s="5" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="P9" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="Q9" s="2" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="5">
         <v>9</v>
       </c>
@@ -1799,8 +2042,14 @@
       <c r="O10" s="5" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="P10" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="Q10" s="1" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -1846,8 +2095,14 @@
       <c r="O11" s="5" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="P11" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="Q11" s="2" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="5">
         <v>11</v>
       </c>
@@ -1893,8 +2148,14 @@
       <c r="O12" s="5" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="P12" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="Q12" s="2" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="5">
         <v>12</v>
       </c>
@@ -1940,8 +2201,14 @@
       <c r="O13" s="5" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="P13" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="Q13" s="2" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="5">
         <v>13</v>
       </c>
@@ -1987,8 +2254,14 @@
       <c r="O14" s="5" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="P14" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="Q14" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="5">
         <v>14</v>
       </c>
@@ -2034,8 +2307,14 @@
       <c r="O15" s="5" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="P15" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="Q15" s="2" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="5">
         <v>15</v>
       </c>
@@ -2081,8 +2360,14 @@
       <c r="O16" s="5" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="P16" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="Q16" s="2" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="5">
         <v>16</v>
       </c>
@@ -2128,8 +2413,14 @@
       <c r="O17" s="5" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="P17" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="Q17" s="2" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="5">
         <v>17</v>
       </c>
@@ -2175,8 +2466,14 @@
       <c r="O18" s="5" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="P18" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="Q18" s="2" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="5">
         <v>18</v>
       </c>
@@ -2222,8 +2519,14 @@
       <c r="O19" s="5" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="P19" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="Q19" s="1" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="5">
         <v>19</v>
       </c>
@@ -2269,8 +2572,14 @@
       <c r="O20" s="5" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="P20" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="Q20" s="2" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="5">
         <v>20</v>
       </c>
@@ -2316,8 +2625,14 @@
       <c r="O21" s="5" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="P21" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="Q21" s="2" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="5">
         <v>21</v>
       </c>
@@ -2363,8 +2678,14 @@
       <c r="O22" s="5" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="P22" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="Q22" s="2" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="5">
         <v>22</v>
       </c>
@@ -2410,8 +2731,14 @@
       <c r="O23" s="5" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="P23" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="Q23" s="2" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="5">
         <v>23</v>
       </c>
@@ -2457,8 +2784,14 @@
       <c r="O24" s="5" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="P24" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="Q24" s="2" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="5">
         <v>24</v>
       </c>
@@ -2504,8 +2837,14 @@
       <c r="O25" s="5" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="P25" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="Q25" s="1" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="5">
         <v>25</v>
       </c>
@@ -2551,8 +2890,14 @@
       <c r="O26" s="5" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="P26" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="Q26" s="2" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="5">
         <v>26</v>
       </c>
@@ -2598,8 +2943,14 @@
       <c r="O27" s="5" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="P27" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="Q27" s="1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="5">
         <v>27</v>
       </c>
@@ -2645,8 +2996,14 @@
       <c r="O28" s="5" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="P28" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="Q28" s="1" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="5">
         <v>28</v>
       </c>
@@ -2692,8 +3049,14 @@
       <c r="O29" s="5" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="P29" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="Q29" s="2" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="5">
         <v>29</v>
       </c>
@@ -2739,8 +3102,14 @@
       <c r="O30" s="5" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="P30" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="Q30" s="2" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="5">
         <v>30</v>
       </c>
@@ -2786,8 +3155,14 @@
       <c r="O31" s="5" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="P31" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="Q31" s="2" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="5">
         <v>31</v>
       </c>
@@ -2833,8 +3208,14 @@
       <c r="O32" s="5" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="P32" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="Q32" s="2" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="5">
         <v>32</v>
       </c>
@@ -2880,8 +3261,14 @@
       <c r="O33" s="5" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="P33" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="Q33" s="2" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="5">
         <v>33</v>
       </c>
@@ -2927,8 +3314,14 @@
       <c r="O34" s="5" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="P34" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="Q34" s="2" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="5">
         <v>34</v>
       </c>
@@ -2974,8 +3367,14 @@
       <c r="O35" s="5" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="P35" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="Q35" s="2" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="5">
         <v>35</v>
       </c>
@@ -3021,8 +3420,14 @@
       <c r="O36" s="5" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="P36" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="Q36" s="2" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="5">
         <v>36</v>
       </c>
@@ -3068,8 +3473,17 @@
       <c r="O37" s="5" t="s">
         <v>183</v>
       </c>
+      <c r="P37" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="Q37" s="2" t="s">
+        <v>270</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="P3" r:id="rId1" xr:uid="{11219FA1-B4DB-4556-A9EA-27B1B66B97F9}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>